<commit_message>
Updated pandas append to concat.
</commit_message>
<xml_diff>
--- a/Databases/QuestionDB.xlsx
+++ b/Databases/QuestionDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\OneDrive\Documents\GitHub\QualificationPractice\Databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e3a85a737daae704/Documents/GitHub/QualificationPractice/Databases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C1B436-F2C3-4837-975F-2D6BA680D598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="13_ncr:1_{69C1B436-F2C3-4837-975F-2D6BA680D598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2683F786-F1AC-4F9C-A38C-4BEC106D8190}"/>
   <bookViews>
-    <workbookView xWindow="5925" yWindow="1733" windowWidth="21600" windowHeight="11392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2263" yWindow="2263" windowWidth="27823" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QuestionDB" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="188">
   <si>
     <t>Question ID</t>
   </si>
@@ -40,90 +40,15 @@
     <t>Skills String</t>
   </si>
   <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb01</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb02</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb03</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb04</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb05</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb06</t>
-  </si>
-  <si>
     <t>0;1</t>
   </si>
   <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb07</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb08</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb09</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb10</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb11</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb12</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb13</t>
-  </si>
-  <si>
     <t>0;1;2</t>
   </si>
   <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb14</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb15</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb16</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb17</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Answers/Nayfeh_ch01_a18.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb18</t>
-  </si>
-  <si>
     <t>1;2</t>
   </si>
   <si>
-    <t xml:space="preserve"> Answers/Nayfeh_ch01_a19.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb19</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Answers/Nayfeh_ch01_a20.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb20</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Answers/Nayfeh_ch01_a21.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and Magnetism Nafeh Ch01 Pb21</t>
-  </si>
-  <si>
     <t>Questions/Nayfeh_ch01_q21.png</t>
   </si>
   <si>
@@ -464,13 +389,208 @@
   </si>
   <si>
     <t>3;9</t>
+  </si>
+  <si>
+    <t>Answers/Landau_ch05_a01.png</t>
+  </si>
+  <si>
+    <t>Questions/Landau_ch05_q01.png</t>
+  </si>
+  <si>
+    <t>Questions/Landau_ch05_q02.png</t>
+  </si>
+  <si>
+    <t>Questions/Landau_ch05_q03.png</t>
+  </si>
+  <si>
+    <t>Questions/Landau_ch05_q04.png</t>
+  </si>
+  <si>
+    <t>Questions/Landau_ch05_q05.png</t>
+  </si>
+  <si>
+    <t>Questions/Landau_ch05_q06.png</t>
+  </si>
+  <si>
+    <t>Answers/Landau_ch05_a02.png</t>
+  </si>
+  <si>
+    <t>Answers/Landau_ch05_a03.png</t>
+  </si>
+  <si>
+    <t>Answers/Landau_ch05_a04.png</t>
+  </si>
+  <si>
+    <t>Answers/Landau_ch05_a05.png</t>
+  </si>
+  <si>
+    <t>Answers/Landau_ch05_a06.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q01.png</t>
+  </si>
+  <si>
+    <t>Mechanics Third Edition Ch05 Pb 1</t>
+  </si>
+  <si>
+    <t>Mechanics Third Edition Ch05 Pb 2</t>
+  </si>
+  <si>
+    <t>Mechanics Third Edition Ch05 Pb 4</t>
+  </si>
+  <si>
+    <t>Mechanics Third Edition Ch05 Pb 3a</t>
+  </si>
+  <si>
+    <t>Mechanics Third Edition Ch05 Pb 3b</t>
+  </si>
+  <si>
+    <t>Mechanics Third Edition Ch05 Pb 3c</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb01</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a01.png</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb03</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb05</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb07</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb09</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb11</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb13</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb15</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q03.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q05.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q07.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q09.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q11.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q13.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q15.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q17.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q19.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q21.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q23.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q25.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q27.png</t>
+  </si>
+  <si>
+    <t>Questions/Nayfeh_ch02_q29.png</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb17</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb19</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb21</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb23</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb25</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb27</t>
+  </si>
+  <si>
+    <t>Fundamental os Statistical and Thermal Physics Reif Ch02 Pb29</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a03.png</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a05.png</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a07.png</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a09.png</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a15.png</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a13.png</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a11.png</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a17.png</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a19.png</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a21.png</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a23.png</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a25.png</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a27.png</t>
+  </si>
+  <si>
+    <t>Answers/Nayfeh_ch02_a29.png</t>
+  </si>
+  <si>
+    <t>12;16</t>
+  </si>
+  <si>
+    <t>16;17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -601,6 +721,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1304,20 +1430,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="22.08984375" customWidth="1"/>
-    <col min="4" max="4" width="33.26953125" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.07421875" customWidth="1"/>
+    <col min="4" max="4" width="33.23046875" customWidth="1"/>
+    <col min="5" max="5" width="41.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1337,7 +1463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1345,19 +1471,19 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1365,19 +1491,19 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1385,19 +1511,19 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1405,19 +1531,19 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1425,19 +1551,19 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1445,19 +1571,19 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1465,19 +1591,19 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1485,19 +1611,19 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1505,19 +1631,19 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
         <v>63</v>
       </c>
-      <c r="E10" t="s">
-        <v>88</v>
-      </c>
       <c r="F10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1525,19 +1651,19 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1545,19 +1671,19 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1565,19 +1691,19 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1585,19 +1711,19 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" t="s">
-        <v>67</v>
-      </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1605,19 +1731,19 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1625,19 +1751,19 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1645,19 +1771,19 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1665,19 +1791,19 @@
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="F18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1685,19 +1811,19 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1705,19 +1831,19 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1725,19 +1851,19 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1745,19 +1871,19 @@
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1765,19 +1891,19 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="D23" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="E23" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="F23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1785,19 +1911,19 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="F24">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1805,19 +1931,19 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="E25" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F25">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1825,19 +1951,19 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="E26" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="F26">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1845,19 +1971,19 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="E27" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="F27">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1865,19 +1991,19 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="E28" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="F28">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1885,19 +2011,19 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="E29" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="F29">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1905,19 +2031,19 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="F30">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1925,19 +2051,19 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="D31" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="E31" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="F31">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1945,19 +2071,19 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="E32" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="F32" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1965,19 +2091,19 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="E33" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="F33" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1985,19 +2111,19 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="E34" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="F34" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2005,19 +2131,19 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="E35" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="F35">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2025,19 +2151,19 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="D36" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="E36" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="F36">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2045,19 +2171,19 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="E37" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="F37" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2065,19 +2191,440 @@
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="D38" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" t="s">
+        <v>119</v>
+      </c>
+      <c r="F38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39" t="s">
+        <v>136</v>
+      </c>
+      <c r="F39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" t="s">
+        <v>130</v>
+      </c>
+      <c r="E40" t="s">
+        <v>137</v>
+      </c>
+      <c r="F40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" t="s">
+        <v>131</v>
+      </c>
+      <c r="E41" t="s">
+        <v>139</v>
+      </c>
+      <c r="F41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>127</v>
+      </c>
+      <c r="D42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" t="s">
+        <v>140</v>
+      </c>
+      <c r="F42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
         <v>128</v>
       </c>
-      <c r="E38" t="s">
+      <c r="D43" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" t="s">
+        <v>141</v>
+      </c>
+      <c r="F43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" t="s">
+        <v>138</v>
+      </c>
+      <c r="F44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>135</v>
+      </c>
+      <c r="D45" t="s">
+        <v>143</v>
+      </c>
+      <c r="E45" t="s">
+        <v>142</v>
+      </c>
+      <c r="F45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>151</v>
+      </c>
+      <c r="D46" t="s">
+        <v>172</v>
+      </c>
+      <c r="E46" t="s">
         <v>144</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F46">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>152</v>
+      </c>
+      <c r="D47" t="s">
+        <v>173</v>
+      </c>
+      <c r="E47" t="s">
+        <v>145</v>
+      </c>
+      <c r="F47">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" t="s">
+        <v>174</v>
+      </c>
+      <c r="E48" t="s">
+        <v>146</v>
+      </c>
+      <c r="F48">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>154</v>
+      </c>
+      <c r="D49" t="s">
+        <v>175</v>
+      </c>
+      <c r="E49" t="s">
         <v>147</v>
       </c>
+      <c r="F49">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>155</v>
+      </c>
+      <c r="D50" t="s">
+        <v>178</v>
+      </c>
+      <c r="E50" t="s">
+        <v>148</v>
+      </c>
+      <c r="F50">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" t="s">
+        <v>177</v>
+      </c>
+      <c r="E51" t="s">
+        <v>149</v>
+      </c>
+      <c r="F51">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>157</v>
+      </c>
+      <c r="D52" t="s">
+        <v>176</v>
+      </c>
+      <c r="E52" t="s">
+        <v>150</v>
+      </c>
+      <c r="F52">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>158</v>
+      </c>
+      <c r="D53" t="s">
+        <v>179</v>
+      </c>
+      <c r="E53" t="s">
+        <v>165</v>
+      </c>
+      <c r="F53">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" t="s">
+        <v>180</v>
+      </c>
+      <c r="E54" t="s">
+        <v>166</v>
+      </c>
+      <c r="F54" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
+      </c>
+      <c r="C55" t="s">
+        <v>160</v>
+      </c>
+      <c r="D55" t="s">
+        <v>181</v>
+      </c>
+      <c r="E55" t="s">
+        <v>167</v>
+      </c>
+      <c r="F55" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>161</v>
+      </c>
+      <c r="D56" t="s">
+        <v>182</v>
+      </c>
+      <c r="E56" t="s">
+        <v>168</v>
+      </c>
+      <c r="F56">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
+        <v>162</v>
+      </c>
+      <c r="D57" t="s">
+        <v>183</v>
+      </c>
+      <c r="E57" t="s">
+        <v>169</v>
+      </c>
+      <c r="F57">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>3</v>
+      </c>
+      <c r="C58" t="s">
+        <v>163</v>
+      </c>
+      <c r="D58" t="s">
+        <v>184</v>
+      </c>
+      <c r="E58" t="s">
+        <v>170</v>
+      </c>
+      <c r="F58">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>164</v>
+      </c>
+      <c r="D59" t="s">
+        <v>185</v>
+      </c>
+      <c r="E59" t="s">
+        <v>171</v>
+      </c>
+      <c r="F59">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>